<commit_message>
Set print range and page orientation on yearly bike report
Closes #238
</commit_message>
<xml_diff>
--- a/comptages/report/template_yearly_bike.xlsx
+++ b/comptages/report/template_yearly_bike.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Data_count" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,13 +19,14 @@
     <sheet name="CAT" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">AN_GR!$A$1:$Z$62</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">AN_TE!$A$1:$N$76</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm.Print_Area" vbProcedure="false">CAT!$A$1:$K$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">CV_LV!$A$1:$K$58</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">AN_GR!$A$7:$K$59</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">AN_TE!$A$1:$N$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm.Print_Area" vbProcedure="false">CAT!$A$1:$K$11,CAT!$A$1:$K$55</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">CV_LV!$A$1:$K$58</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">AN_GR!$A$1:$K$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0" vbProcedure="false">AN_GR!$A$1:$K$11,AN_GR!$A$1:$K$55</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm.Print_Area" vbProcedure="false">CAT!$A$1:$K$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0" vbProcedure="false">AN_GR!$A$1:$K$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0" vbProcedure="false">AN_GR!$A$1:$K$11,AN_GR!$A$1:$K$55</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm.Print_Area" vbProcedure="false">CAT!$A$1:$K$11,CAT!$A$1:$K$59</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="173">
   <si>
     <t xml:space="preserve">Data of the count</t>
   </si>
@@ -352,6 +353,9 @@
   </si>
   <si>
     <t xml:space="preserve">décembre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tfla</t>
   </si>
   <si>
     <t xml:space="preserve">Courbe de variation annuelle</t>
@@ -1373,7 +1377,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart82.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1522,8 +1526,8 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="0"/>
-        <c:axId val="49204118"/>
-        <c:axId val="92880767"/>
+        <c:axId val="71537675"/>
+        <c:axId val="84287301"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1817,11 +1821,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="49204118"/>
-        <c:axId val="92880767"/>
+        <c:axId val="71537675"/>
+        <c:axId val="84287301"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49204118"/>
+        <c:axId val="71537675"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1887,7 +1891,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92880767"/>
+        <c:crossAx val="84287301"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1895,7 +1899,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92880767"/>
+        <c:axId val="84287301"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1971,7 +1975,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49204118"/>
+        <c:crossAx val="71537675"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2023,7 +2027,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4299,11 +4303,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="55217692"/>
-        <c:axId val="36118157"/>
+        <c:axId val="46638155"/>
+        <c:axId val="80419887"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55217692"/>
+        <c:axId val="46638155"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4331,7 +4335,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36118157"/>
+        <c:crossAx val="80419887"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4339,7 +4343,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36118157"/>
+        <c:axId val="80419887"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4376,7 +4380,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55217692"/>
+        <c:crossAx val="46638155"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4424,7 +4428,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4546,11 +4550,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="15631478"/>
-        <c:axId val="64773851"/>
+        <c:axId val="73001233"/>
+        <c:axId val="19408962"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="15631478"/>
+        <c:axId val="73001233"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4578,7 +4582,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64773851"/>
+        <c:crossAx val="19408962"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4586,7 +4590,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64773851"/>
+        <c:axId val="19408962"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4623,7 +4627,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15631478"/>
+        <c:crossAx val="73001233"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4671,7 +4675,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4851,7 +4855,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4998,8 +5002,8 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="0"/>
-        <c:axId val="18136360"/>
-        <c:axId val="16596523"/>
+        <c:axId val="49361410"/>
+        <c:axId val="24963102"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5289,11 +5293,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="18136360"/>
-        <c:axId val="16596523"/>
+        <c:axId val="49361410"/>
+        <c:axId val="24963102"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="18136360"/>
+        <c:axId val="49361410"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5359,7 +5363,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16596523"/>
+        <c:crossAx val="24963102"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5367,7 +5371,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16596523"/>
+        <c:axId val="24963102"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5409,7 +5413,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18136360"/>
+        <c:crossAx val="49361410"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5461,7 +5465,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart87.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5608,8 +5612,8 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="0"/>
-        <c:axId val="37486215"/>
-        <c:axId val="97711295"/>
+        <c:axId val="96978235"/>
+        <c:axId val="53239184"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5899,11 +5903,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="37486215"/>
-        <c:axId val="97711295"/>
+        <c:axId val="96978235"/>
+        <c:axId val="53239184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37486215"/>
+        <c:axId val="96978235"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5969,7 +5973,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97711295"/>
+        <c:crossAx val="53239184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5977,7 +5981,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97711295"/>
+        <c:axId val="53239184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6019,7 +6023,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37486215"/>
+        <c:crossAx val="96978235"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6071,7 +6075,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart88.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6147,6 +6151,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -6208,6 +6213,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -6269,6 +6275,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -6297,17 +6304,17 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="18959293"/>
-        <c:axId val="82322664"/>
+        <c:axId val="24653214"/>
+        <c:axId val="41931266"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="18959293"/>
+        <c:axId val="24653214"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6329,7 +6336,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82322664"/>
+        <c:crossAx val="41931266"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6337,7 +6344,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82322664"/>
+        <c:axId val="41931266"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6352,7 +6359,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6374,7 +6381,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18959293"/>
+        <c:crossAx val="24653214"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6422,7 +6429,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart89.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6496,6 +6503,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -6557,6 +6565,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -6618,6 +6627,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -6679,6 +6689,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -6707,17 +6718,17 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="99229431"/>
-        <c:axId val="47363245"/>
+        <c:axId val="67137129"/>
+        <c:axId val="62120218"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="99229431"/>
+        <c:axId val="67137129"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6739,7 +6750,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47363245"/>
+        <c:crossAx val="62120218"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6747,7 +6758,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47363245"/>
+        <c:axId val="62120218"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6762,7 +6773,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6784,7 +6795,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99229431"/>
+        <c:crossAx val="67137129"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6843,9 +6854,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>583560</xdr:colOff>
+      <xdr:colOff>583200</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>156960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6854,7 +6865,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="2676600"/>
-        <a:ext cx="6903000" cy="2910600"/>
+        <a:ext cx="6902640" cy="2910240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6877,10 +6888,10 @@
       <xdr:rowOff>66960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>537480</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>341280</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>28080</xdr:rowOff>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6889,7 +6900,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="49320" y="1924200"/>
-        <a:ext cx="6775920" cy="3037680"/>
+        <a:ext cx="16439760" cy="3037320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6901,16 +6912,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>400320</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>51480</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>519840</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>48240</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>297360</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>54360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6918,8 +6929,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3614400" y="5531760"/>
-        <a:ext cx="3193200" cy="1555200"/>
+        <a:off x="8934840" y="5477760"/>
+        <a:ext cx="7510320" cy="2101320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6937,10 +6948,10 @@
       <xdr:rowOff>40680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>69480</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>615600</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>43560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6949,7 +6960,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="52560" y="5460120"/>
-        <a:ext cx="3231000" cy="1683720"/>
+        <a:ext cx="8125560" cy="2108160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6961,16 +6972,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>414360</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>55080</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>525240</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>264240</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6978,8 +6989,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3628440" y="7963200"/>
-        <a:ext cx="3184560" cy="1342800"/>
+        <a:off x="8938440" y="7920000"/>
+        <a:ext cx="7473600" cy="2066400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6997,10 +7008,10 @@
       <xdr:rowOff>104400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>59400</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571680</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7009,7 +7020,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="29880" y="7952760"/>
-        <a:ext cx="3243600" cy="1367640"/>
+        <a:ext cx="8104320" cy="2044440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7027,15 +7038,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>155880</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>573840</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>417960</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>139320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7043,8 +7054,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4671360" y="1895760"/>
-        <a:ext cx="2876400" cy="1343160"/>
+        <a:off x="4759200" y="1906920"/>
+        <a:ext cx="4568400" cy="1870920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7057,15 +7068,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>198360</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>353160</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>561960</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>572400</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7073,8 +7084,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4098960" y="3360240"/>
-        <a:ext cx="3436920" cy="2981160"/>
+        <a:off x="4253760" y="3975840"/>
+        <a:ext cx="5228280" cy="4534920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7094,11 +7105,11 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="119.13"/>
@@ -7227,7 +7238,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -10192,7 +10203,7 @@
       <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -11002,7 +11013,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -11095,7 +11106,7 @@
       <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -11154,28 +11165,28 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="4" t="n">
         <f aca="false">SUM(B5:B9)</f>
         <v>39871</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="4" t="n">
         <f aca="false">B5</f>
         <v>36905</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="4" t="n">
         <f aca="false">SUM(B6:B9)</f>
         <v>2966</v>
       </c>
@@ -11198,11 +11209,11 @@
   </sheetPr>
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N25" activeCellId="0" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="8.71"/>
@@ -11607,7 +11618,7 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
 Département du développement
-territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+territorial et de l'environnement&amp;CComptage mobilité douce&amp;R&amp;8Service des ponts et chaussées
 Bureau signalisation et circulation
 Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
@@ -11623,11 +11634,11 @@
   </sheetPr>
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K43" activeCellId="0" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="9.59"/>
@@ -13638,7 +13649,7 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
 Département du développement
-territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+territorial et de l'environnement&amp;CComptage mobilité douce&amp;R&amp;8Service des ponts et chaussées
 Bureau signalisation et circulation
 Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
@@ -13651,13 +13662,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I60" activeCellId="0" sqref="I60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="8.71"/>
@@ -13676,12 +13687,14 @@
         <f aca="false">Data_count!B4</f>
         <v> </v>
       </c>
-      <c r="G2" s="12" t="str">
+      <c r="G2" s="0"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="0"/>
+      <c r="N2" s="12" t="str">
         <f aca="false">Data_count!B5</f>
         <v> </v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10" t="str">
+      <c r="Z2" s="10" t="str">
         <f aca="false">Data_count!B6</f>
         <v> </v>
       </c>
@@ -13693,7 +13706,8 @@
       </c>
       <c r="G3" s="12"/>
       <c r="J3" s="9"/>
-      <c r="K3" s="13" t="str">
+      <c r="K3" s="0"/>
+      <c r="Z3" s="13" t="str">
         <f aca="false">Data_count!B7</f>
         <v> </v>
       </c>
@@ -13707,7 +13721,8 @@
         <v> </v>
       </c>
       <c r="J4" s="9"/>
-      <c r="K4" s="13" t="str">
+      <c r="K4" s="0"/>
+      <c r="Z4" s="13" t="str">
         <f aca="false">Data_count!B8</f>
         <v> </v>
       </c>
@@ -13721,7 +13736,8 @@
         <v> </v>
       </c>
       <c r="J5" s="9"/>
-      <c r="K5" s="13" t="str">
+      <c r="K5" s="0"/>
+      <c r="Z5" s="13" t="str">
         <f aca="false">Data_count!B9</f>
         <v> </v>
       </c>
@@ -13732,41 +13748,46 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11"/>
+      <c r="A7" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="C7" s="15"/>
-      <c r="G7" s="16" t="str">
+      <c r="G7" s="0"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="N7" s="16" t="str">
         <f aca="false">Data_count!B11</f>
         <v> </v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="59" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="59" t="s">
-        <v>106</v>
-      </c>
-      <c r="G32" s="59" t="s">
         <v>107</v>
+      </c>
+      <c r="G32" s="0"/>
+      <c r="O32" s="59" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="G47" s="59" t="s">
         <v>109</v>
       </c>
+      <c r="G47" s="0"/>
+      <c r="O47" s="59" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0"/>
+      <c r="A55" s="4"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0"/>
+      <c r="A78" s="4"/>
     </row>
     <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -13821,11 +13842,11 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.96805555555556" bottom="0.472222222222222" header="0.708333333333333" footer="0.196527777777778"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
 Département du développement
-territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+territorial et de l'environnement&amp;CComptage mobilité douce&amp;R&amp;8Service des ponts et chaussées
 Bureau signalisation et circulation
 Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
@@ -13839,13 +13860,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O17" activeCellId="0" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.96"/>
@@ -13867,12 +13888,14 @@
         <f aca="false">Data_count!B4</f>
         <v> </v>
       </c>
-      <c r="G2" s="12" t="str">
+      <c r="G2" s="0"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="0"/>
+      <c r="N2" s="12" t="str">
         <f aca="false">Data_count!B5</f>
         <v> </v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10" t="str">
+      <c r="Z2" s="10" t="str">
         <f aca="false">Data_count!B6</f>
         <v> </v>
       </c>
@@ -13884,7 +13907,8 @@
       </c>
       <c r="G3" s="12"/>
       <c r="J3" s="9"/>
-      <c r="K3" s="13" t="str">
+      <c r="K3" s="0"/>
+      <c r="Z3" s="13" t="str">
         <f aca="false">Data_count!B7</f>
         <v> </v>
       </c>
@@ -13898,7 +13922,8 @@
         <v> </v>
       </c>
       <c r="J4" s="9"/>
-      <c r="K4" s="13" t="str">
+      <c r="K4" s="0"/>
+      <c r="Z4" s="13" t="str">
         <f aca="false">Data_count!B8</f>
         <v> </v>
       </c>
@@ -13912,7 +13937,8 @@
         <v> </v>
       </c>
       <c r="J5" s="9"/>
-      <c r="K5" s="13" t="str">
+      <c r="K5" s="0"/>
+      <c r="Z5" s="13" t="str">
         <f aca="false">Data_count!B9</f>
         <v> </v>
       </c>
@@ -13925,16 +13951,17 @@
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="11"/>
       <c r="C7" s="15"/>
-      <c r="G7" s="16" t="str">
+      <c r="G7" s="0"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="N7" s="16" t="str">
         <f aca="false">Data_count!B11</f>
         <v> </v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="59" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F9" s="60" t="n">
         <f aca="false">Data_class!B10</f>
@@ -13954,243 +13981,175 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="63" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B11" s="64" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D11" s="65"/>
       <c r="E11" s="66" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F11" s="66"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="67" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C12" s="68" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D12" s="68"/>
       <c r="E12" s="69" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F12" s="69"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="67" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C13" s="68" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D13" s="68"/>
       <c r="E13" s="69" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F13" s="69"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="67" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C14" s="68" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D14" s="68"/>
       <c r="E14" s="69" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F14" s="69"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="70" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B15" s="71" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C15" s="72" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D15" s="72"/>
       <c r="E15" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F15" s="73"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="74" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" s="75" t="s">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="74" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="75" t="s">
+      <c r="B24" s="75" t="s">
         <v>132</v>
       </c>
-      <c r="D20" s="75" t="s">
+      <c r="C24" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="76" t="s">
+      <c r="D24" s="75" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="77" t="s">
+      <c r="E24" s="76" t="s">
         <v>135</v>
-      </c>
-      <c r="B21" s="78" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="E21" s="79" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="77" t="s">
-        <v>137</v>
-      </c>
-      <c r="B22" s="78" t="s">
-        <v>136</v>
-      </c>
-      <c r="C22" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="E22" s="79" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="77" t="s">
-        <v>138</v>
-      </c>
-      <c r="B23" s="78" t="s">
-        <v>136</v>
-      </c>
-      <c r="C23" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="E23" s="79" t="n">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="77" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="78" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="78" t="n">
-        <v>2</v>
-      </c>
-      <c r="E24" s="79" t="n">
-        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="77" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B25" s="78" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C25" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="78" t="n">
         <v>2</v>
       </c>
-      <c r="D25" s="78" t="n">
-        <v>3</v>
-      </c>
-      <c r="E25" s="79" t="s">
-        <v>141</v>
+      <c r="E25" s="79" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="77" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B26" s="78" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C26" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="78" t="n">
         <v>2</v>
       </c>
-      <c r="D26" s="78" t="n">
-        <v>3</v>
-      </c>
-      <c r="E26" s="79" t="s">
-        <v>144</v>
+      <c r="E26" s="79" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="77" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B27" s="78" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C27" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="78" t="n">
         <v>2</v>
       </c>
-      <c r="D27" s="78" t="n">
-        <v>3</v>
-      </c>
-      <c r="E27" s="79" t="s">
-        <v>147</v>
+      <c r="E27" s="79" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="77" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B28" s="78" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C28" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="78" t="n">
         <v>2</v>
       </c>
-      <c r="D28" s="78" t="n">
-        <v>3</v>
-      </c>
-      <c r="E28" s="79" t="s">
-        <v>149</v>
+      <c r="E28" s="79" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="77" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B29" s="78" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C29" s="78" t="n">
         <v>2</v>
@@ -14199,117 +14158,117 @@
         <v>3</v>
       </c>
       <c r="E29" s="79" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="77" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="B30" s="78" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C30" s="78" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="78" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30" s="79" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="77" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="78" t="n">
-        <v>115</v>
+        <v>146</v>
+      </c>
+      <c r="B31" s="78" t="s">
+        <v>147</v>
       </c>
       <c r="C31" s="78" t="n">
         <v>2</v>
       </c>
       <c r="D31" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="79" t="n">
-        <v>185</v>
+        <v>3</v>
+      </c>
+      <c r="E31" s="79" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="77" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B32" s="78" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C32" s="78" t="n">
         <v>2</v>
       </c>
       <c r="D32" s="78" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E32" s="79" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="77" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="B33" s="78" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C33" s="78" t="n">
         <v>2</v>
       </c>
       <c r="D33" s="78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33" s="79" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="77" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B34" s="78" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C34" s="78" t="n">
         <v>2</v>
       </c>
       <c r="D34" s="78" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E34" s="79" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="77" t="s">
-        <v>161</v>
-      </c>
-      <c r="B35" s="78" t="s">
-        <v>162</v>
+        <v>33</v>
+      </c>
+      <c r="B35" s="78" t="n">
+        <v>115</v>
       </c>
       <c r="C35" s="78" t="n">
         <v>2</v>
       </c>
       <c r="D35" s="78" t="n">
-        <v>4</v>
-      </c>
-      <c r="E35" s="79" t="s">
-        <v>163</v>
+        <v>1</v>
+      </c>
+      <c r="E35" s="79" t="n">
+        <v>185</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="77" t="s">
-        <v>164</v>
+        <v>113</v>
       </c>
       <c r="B36" s="78" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C36" s="78" t="n">
         <v>2</v>
@@ -14318,15 +14277,15 @@
         <v>1</v>
       </c>
       <c r="E36" s="79" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="77" t="s">
-        <v>167</v>
+        <v>125</v>
       </c>
       <c r="B37" s="78" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C37" s="78" t="n">
         <v>2</v>
@@ -14335,36 +14294,100 @@
         <v>4</v>
       </c>
       <c r="E37" s="79" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="77" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" s="78" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="D38" s="78" t="n">
+        <v>4</v>
+      </c>
+      <c r="E38" s="79" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="77" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" s="78" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="D39" s="78" t="n">
+        <v>4</v>
+      </c>
+      <c r="E39" s="79" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="77" t="s">
+        <v>165</v>
+      </c>
+      <c r="B40" s="78" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="D40" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="79" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="78" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="80" t="s">
-        <v>127</v>
-      </c>
-      <c r="B38" s="81" t="s">
+      <c r="C41" s="78" t="n">
+        <v>2</v>
+      </c>
+      <c r="D41" s="78" t="n">
+        <v>4</v>
+      </c>
+      <c r="E41" s="79" t="s">
         <v>170</v>
       </c>
-      <c r="C38" s="81" t="n">
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="80" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="81" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="81" t="n">
         <v>3</v>
       </c>
-      <c r="D38" s="81" t="n">
+      <c r="D42" s="81" t="n">
         <v>5</v>
       </c>
-      <c r="E38" s="82" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="59"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="59"/>
-    </row>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E42" s="82" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="59"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="59"/>
+    </row>
     <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -14426,7 +14449,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.96805555555556" bottom="0.472222222222222" header="0.708333333333333" footer="0.196527777777778"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
 Département du développement

</xml_diff>

<commit_message>
ajout de filtres et  légères adaptations
</commit_message>
<xml_diff>
--- a/comptages/report/template_yearly_bike.xlsx
+++ b/comptages/report/template_yearly_bike.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="214">
   <si>
     <t>Data of the count</t>
   </si>
@@ -226,9 +226,6 @@
     <t>velo</t>
   </si>
   <si>
-    <t>autres</t>
-  </si>
-  <si>
     <t>Direction 1 :</t>
   </si>
   <si>
@@ -662,6 +659,24 @@
   </si>
   <si>
     <t>total MD</t>
+  </si>
+  <si>
+    <t>trash</t>
+  </si>
+  <si>
+    <t>Non MD !</t>
+  </si>
+  <si>
+    <t>autres MD</t>
+  </si>
+  <si>
+    <t>Inconnu</t>
+  </si>
+  <si>
+    <t>Piéton</t>
+  </si>
+  <si>
+    <t>Voiture</t>
   </si>
 </sst>
 </file>
@@ -4406,7 +4421,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data_class!$A$14</c:f>
+              <c:f>Data_class!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4461,7 +4476,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data_class!$B$14</c:f>
+              <c:f>Data_class!$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -4482,11 +4497,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data_class!$A$15</c:f>
+              <c:f>Data_class!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>autres</c:v>
+                  <c:v>autres MD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4537,7 +4552,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data_class!$B$15</c:f>
+              <c:f>Data_class!$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -5841,7 +5856,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -5874,10 +5889,10 @@
         <v>28</v>
       </c>
       <c r="P3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q3" t="s">
         <v>204</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -6536,10 +6551,10 @@
         <v>28</v>
       </c>
       <c r="P20" s="79" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q20" s="79" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
@@ -7293,7 +7308,7 @@
         <v>0</v>
       </c>
       <c r="H37" s="50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -7349,7 +7364,7 @@
         <v>28</v>
       </c>
       <c r="O39" s="50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
@@ -14381,10 +14396,10 @@
         <v>56</v>
       </c>
       <c r="F4" s="79" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G4" s="79" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -15754,18 +15769,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" s="79" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="79" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -15773,17 +15788,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="74" t="e">
-        <f t="shared" ref="C4:C9" si="0">B4/$B$11</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" ref="C4:C9" si="0">B4/$B$20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E4" s="82" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -15792,8 +15810,11 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -15802,8 +15823,11 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -15812,8 +15836,11 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -15822,8 +15849,11 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -15832,48 +15862,160 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="E9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="79">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="74" t="e">
+        <f t="shared" ref="C10:C12" si="1">B10/$B$20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E10" s="82" t="s">
+        <v>209</v>
+      </c>
+      <c r="F10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="79">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="74" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" s="82" t="s">
+        <v>209</v>
+      </c>
+      <c r="F11" s="79" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="79">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="74" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E12" s="82" t="s">
+        <v>209</v>
+      </c>
+      <c r="F12" s="79" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="79">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="74" t="e">
+        <f t="shared" ref="C13:C18" si="2">B13/$B$20</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="79">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="74" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="79">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="74" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="79">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="74" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="79">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="74" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="79">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="74" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="79" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B11">
-        <f>SUM(B4:B9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>208</v>
-      </c>
-      <c r="B13" s="79">
+      <c r="B20">
+        <f>SUM(B4:B18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" s="79">
         <f>SUM(B5:B9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>62</v>
       </c>
-      <c r="B14">
+      <c r="B23">
         <f>B5</f>
         <v>0</v>
       </c>
-      <c r="C14" s="74" t="e">
-        <f>B14/$B$13</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15">
+      <c r="C23" s="74" t="e">
+        <f>B23/$B$22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24">
         <f>SUM(B6:B9)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="74" t="e">
-        <f>B15/$B$13</f>
+      <c r="C24" s="74" t="e">
+        <f>B24/$B$22</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -15941,7 +16083,7 @@
     </row>
     <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="9">
         <f>Data_count!B13</f>
@@ -15955,7 +16097,7 @@
     </row>
     <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="9">
         <f>Data_count!B14</f>
@@ -15994,20 +16136,20 @@
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="90" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="91"/>
       <c r="E9" s="89"/>
       <c r="F9" s="88" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G9" s="89"/>
       <c r="H9" s="92" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I9" s="89"/>
       <c r="J9" s="83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K9" s="84"/>
     </row>
@@ -16021,31 +16163,31 @@
         <v>55</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>55</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>55</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J10" s="16" t="s">
         <v>55</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
       <c r="B11" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="20">
         <f>D11+E11</f>
@@ -16075,7 +16217,7 @@
     <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24"/>
       <c r="B12" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="26">
         <f>D12+E12</f>
@@ -16104,14 +16246,14 @@
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="85" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B35" s="86"/>
       <c r="C35" s="86"/>
@@ -16126,7 +16268,7 @@
     </row>
     <row r="36" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="85" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36" s="86"/>
       <c r="C36" s="86"/>
@@ -16144,7 +16286,7 @@
     </row>
     <row r="37" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="85" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="86"/>
       <c r="C37" s="86"/>
@@ -16162,7 +16304,7 @@
     </row>
     <row r="38" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="85" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="86"/>
       <c r="C38" s="86"/>
@@ -16180,7 +16322,7 @@
     </row>
     <row r="39" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="85" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" s="86"/>
       <c r="C39" s="86"/>
@@ -16195,7 +16337,7 @@
     </row>
     <row r="40" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="85" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40" s="86"/>
       <c r="C40" s="86"/>
@@ -16210,7 +16352,7 @@
     </row>
     <row r="41" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" s="86"/>
       <c r="C41" s="86"/>
@@ -16318,7 +16460,7 @@
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="9">
         <f>Data_count!B13</f>
@@ -16331,7 +16473,7 @@
     </row>
     <row r="5" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="9">
         <f>Data_count!B14</f>
@@ -16347,7 +16489,7 @@
       <c r="A6" s="6"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J6" s="4"/>
     </row>
@@ -16380,39 +16522,39 @@
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="C13" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="D13" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="E13" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="F13" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="G13" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="H13" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="I13" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="I13" s="33" t="s">
+      <c r="J13" s="33" t="s">
         <v>90</v>
-      </c>
-      <c r="J13" s="33" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14" s="34"/>
@@ -16432,7 +16574,7 @@
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
@@ -16452,7 +16594,7 @@
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
@@ -16472,7 +16614,7 @@
     </row>
     <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
@@ -16492,7 +16634,7 @@
     </row>
     <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
@@ -16512,7 +16654,7 @@
     </row>
     <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
@@ -16532,7 +16674,7 @@
     </row>
     <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
@@ -16552,7 +16694,7 @@
     </row>
     <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
@@ -16572,7 +16714,7 @@
     </row>
     <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
@@ -16592,7 +16734,7 @@
     </row>
     <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
@@ -16612,7 +16754,7 @@
     </row>
     <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
@@ -16632,7 +16774,7 @@
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
@@ -16652,7 +16794,7 @@
     </row>
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" s="34"/>
       <c r="C26" s="34"/>
@@ -16672,7 +16814,7 @@
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
@@ -16692,7 +16834,7 @@
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
@@ -16712,7 +16854,7 @@
     </row>
     <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B29" s="34"/>
       <c r="C29" s="34"/>
@@ -16732,7 +16874,7 @@
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B30" s="34"/>
       <c r="C30" s="34"/>
@@ -16752,7 +16894,7 @@
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B31" s="34"/>
       <c r="C31" s="34"/>
@@ -16772,7 +16914,7 @@
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B32" s="34"/>
       <c r="C32" s="34"/>
@@ -16792,7 +16934,7 @@
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B33" s="34"/>
       <c r="C33" s="34"/>
@@ -16812,7 +16954,7 @@
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B34" s="34"/>
       <c r="C34" s="34"/>
@@ -16832,7 +16974,7 @@
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B35" s="34"/>
       <c r="C35" s="34"/>
@@ -16852,7 +16994,7 @@
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="34"/>
       <c r="C36" s="34"/>
@@ -16872,7 +17014,7 @@
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="34"/>
       <c r="C37" s="34"/>
@@ -16895,12 +17037,12 @@
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B40" s="34">
         <f t="shared" ref="B40:J40" si="2">SUM(B21:B32)</f>
@@ -16941,7 +17083,7 @@
     </row>
     <row r="41" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B41" s="34">
         <f t="shared" ref="B41:J41" si="3">SUM(B20:B35)</f>
@@ -16982,7 +17124,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B42" s="34">
         <f t="shared" ref="B42:J42" si="4">SUM(B20:B37)</f>
@@ -17023,7 +17165,7 @@
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B43" s="34">
         <f t="shared" ref="B43:J43" si="5">SUM(B14:B37)</f>
@@ -17066,44 +17208,44 @@
     <row r="45" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B47" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="33" t="s">
+      <c r="D47" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="33" t="s">
+      <c r="E47" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="E47" s="33" t="s">
+      <c r="F47" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="F47" s="33" t="s">
+      <c r="G47" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="G47" s="33" t="s">
+      <c r="H47" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="H47" s="33" t="s">
+      <c r="I47" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="I47" s="33" t="s">
+      <c r="J47" s="33" t="s">
         <v>90</v>
-      </c>
-      <c r="J47" s="33" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B48" s="34"/>
       <c r="C48" s="34"/>
@@ -17123,7 +17265,7 @@
     </row>
     <row r="49" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B49" s="34"/>
       <c r="C49" s="34"/>
@@ -17143,7 +17285,7 @@
     </row>
     <row r="50" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B50" s="34"/>
       <c r="C50" s="34"/>
@@ -17163,7 +17305,7 @@
     </row>
     <row r="51" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B51" s="34"/>
       <c r="C51" s="34"/>
@@ -17183,7 +17325,7 @@
     </row>
     <row r="52" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B52" s="34"/>
       <c r="C52" s="34"/>
@@ -17203,7 +17345,7 @@
     </row>
     <row r="53" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B53" s="34"/>
       <c r="C53" s="34"/>
@@ -17223,7 +17365,7 @@
     </row>
     <row r="54" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B54" s="34"/>
       <c r="C54" s="34"/>
@@ -17243,7 +17385,7 @@
     </row>
     <row r="55" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B55" s="34"/>
       <c r="C55" s="34"/>
@@ -17263,7 +17405,7 @@
     </row>
     <row r="56" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B56" s="34"/>
       <c r="C56" s="34"/>
@@ -17283,7 +17425,7 @@
     </row>
     <row r="57" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B57" s="34"/>
       <c r="C57" s="34"/>
@@ -17303,7 +17445,7 @@
     </row>
     <row r="58" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B58" s="34"/>
       <c r="C58" s="34"/>
@@ -17323,7 +17465,7 @@
     </row>
     <row r="59" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B59" s="34"/>
       <c r="C59" s="34"/>
@@ -17404,7 +17546,7 @@
     </row>
     <row r="4" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="9">
         <f>Data_count!B13</f>
@@ -17417,7 +17559,7 @@
     </row>
     <row r="5" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="9">
         <f>Data_count!B14</f>
@@ -17439,20 +17581,20 @@
     </row>
     <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="10"/>
       <c r="J7" s="4"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="F31" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="F31" s="36" t="s">
+      <c r="N31" s="36" t="s">
         <v>136</v>
-      </c>
-      <c r="N31" s="36" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -17466,10 +17608,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="F45" s="36" t="s">
         <v>138</v>
-      </c>
-      <c r="F45" s="36" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -17544,7 +17686,7 @@
     </row>
     <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="9">
         <f>Data_count!B13</f>
@@ -17558,7 +17700,7 @@
     </row>
     <row r="5" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="9">
         <f>Data_count!B14</f>
@@ -17588,18 +17730,18 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F9" s="37">
-        <f>Data_class!B11</f>
+        <f>Data_class!B20</f>
         <v>0</v>
       </c>
       <c r="G9" s="38">
-        <f>Data_class!B14</f>
+        <f>Data_class!B23</f>
         <v>0</v>
       </c>
       <c r="H9" s="39">
-        <f>Data_class!B15</f>
+        <f>Data_class!B24</f>
         <v>0</v>
       </c>
     </row>
@@ -17608,107 +17750,107 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" s="41" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="100" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D11" s="89"/>
       <c r="E11" s="101" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F11" s="84"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="78" t="s">
         <v>144</v>
       </c>
-      <c r="B12" s="78" t="s">
+      <c r="C12" s="95" t="s">
         <v>145</v>
-      </c>
-      <c r="C12" s="95" t="s">
-        <v>146</v>
       </c>
       <c r="D12" s="87"/>
       <c r="E12" s="93" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F12" s="94"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="B13" s="78" t="s">
+      <c r="C13" s="95" t="s">
         <v>149</v>
-      </c>
-      <c r="C13" s="95" t="s">
-        <v>150</v>
       </c>
       <c r="D13" s="87"/>
       <c r="E13" s="93" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F13" s="94"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="C14" s="95" t="s">
         <v>153</v>
-      </c>
-      <c r="C14" s="95" t="s">
-        <v>154</v>
       </c>
       <c r="D14" s="87"/>
       <c r="E14" s="93" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F14" s="94"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="C15" s="98" t="s">
         <v>157</v>
-      </c>
-      <c r="C15" s="98" t="s">
-        <v>158</v>
       </c>
       <c r="D15" s="99"/>
       <c r="E15" s="96" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F15" s="97"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="C23" s="56" t="s">
         <v>161</v>
-      </c>
-      <c r="C23" s="56" t="s">
-        <v>162</v>
       </c>
       <c r="D23" s="56" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B24" s="54" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C24" s="58">
         <v>2</v>
@@ -17717,7 +17859,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -17739,10 +17881,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="45" t="s">
         <v>166</v>
-      </c>
-      <c r="B26" s="45" t="s">
-        <v>167</v>
       </c>
       <c r="C26" s="58">
         <v>2</v>
@@ -17751,15 +17893,15 @@
         <v>1</v>
       </c>
       <c r="E26" s="46" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C27" s="58">
         <v>2</v>
@@ -17768,15 +17910,15 @@
         <v>1</v>
       </c>
       <c r="E27" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="64" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B28" s="45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C28" s="58">
         <v>1</v>
@@ -17790,10 +17932,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="64" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B29" s="45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C29" s="58">
         <v>1</v>
@@ -17807,10 +17949,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="64" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C30" s="58">
         <v>1</v>
@@ -17824,10 +17966,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="64" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B31" s="45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C31" s="58">
         <v>1</v>
@@ -17841,10 +17983,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="69" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32" s="45" t="s">
         <v>175</v>
-      </c>
-      <c r="B32" s="45" t="s">
-        <v>176</v>
       </c>
       <c r="C32" s="58">
         <v>2</v>
@@ -17853,15 +17995,15 @@
         <v>3</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="65" t="s">
+        <v>177</v>
+      </c>
+      <c r="B33" s="45" t="s">
         <v>178</v>
-      </c>
-      <c r="B33" s="45" t="s">
-        <v>179</v>
       </c>
       <c r="C33" s="58">
         <v>2</v>
@@ -17870,15 +18012,15 @@
         <v>3</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="65" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B34" s="45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C34" s="58">
         <v>2</v>
@@ -17887,15 +18029,15 @@
         <v>3</v>
       </c>
       <c r="E34" s="46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="45" t="s">
         <v>183</v>
-      </c>
-      <c r="B35" s="45" t="s">
-        <v>184</v>
       </c>
       <c r="C35" s="58">
         <v>2</v>
@@ -17904,15 +18046,15 @@
         <v>3</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="B36" s="45" t="s">
         <v>186</v>
-      </c>
-      <c r="B36" s="45" t="s">
-        <v>187</v>
       </c>
       <c r="C36" s="58">
         <v>2</v>
@@ -17921,16 +18063,16 @@
         <v>3</v>
       </c>
       <c r="E36" s="46" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J36" s="71"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="67" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" s="45" t="s">
         <v>189</v>
-      </c>
-      <c r="B37" s="45" t="s">
-        <v>190</v>
       </c>
       <c r="C37" s="58">
         <v>2</v>
@@ -17939,16 +18081,16 @@
         <v>4</v>
       </c>
       <c r="E37" s="46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J37" s="71"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="67" t="s">
+        <v>191</v>
+      </c>
+      <c r="B38" s="45" t="s">
         <v>192</v>
-      </c>
-      <c r="B38" s="45" t="s">
-        <v>193</v>
       </c>
       <c r="C38" s="58">
         <v>2</v>
@@ -17957,16 +18099,16 @@
         <v>4</v>
       </c>
       <c r="E38" s="46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J38" s="71"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="67" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B39" s="45" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C39" s="58">
         <v>2</v>
@@ -17975,15 +18117,15 @@
         <v>4</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B40" s="45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C40" s="58">
         <v>2</v>
@@ -17992,15 +18134,15 @@
         <v>4</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="68" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B41" s="47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C41" s="60">
         <v>3</v>
@@ -18009,7 +18151,7 @@
         <v>5</v>
       </c>
       <c r="E41" s="48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>